<commit_message>
Incorporación de Funcion ML/Actualizacion de Requirements
</commit_message>
<xml_diff>
--- a/Bases de datos/Diccionario de Datos STEAM.xlsx
+++ b/Bases de datos/Diccionario de Datos STEAM.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documentos\Mai\Henry\Cursado\P.I. 1\PI_ML_OPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documentos\Mai\Henry\Cursado\P.I. 1\Bases de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F81B28-1E1F-4BC4-A362-CD68C51D843A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6030E9-A82C-45C4-82C5-F3B0561A786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Ejemplos para consultas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
   <si>
     <t>steam_games.gz.json</t>
   </si>
@@ -221,12 +221,78 @@
       <t>userdata</t>
     </r>
   </si>
+  <si>
+    <t>User_id</t>
+  </si>
+  <si>
+    <t>Items_id</t>
+  </si>
+  <si>
+    <t>Developers</t>
+  </si>
+  <si>
+    <t>Años</t>
+  </si>
+  <si>
+    <t>evcentric</t>
+  </si>
+  <si>
+    <t>boydeer</t>
+  </si>
+  <si>
+    <t>tarjla</t>
+  </si>
+  <si>
+    <t>duzim</t>
+  </si>
+  <si>
+    <t>SEGA</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>Rockstar Games</t>
+  </si>
+  <si>
+    <t>Standing Stone Games, LLC</t>
+  </si>
+  <si>
+    <t>Capcom U.S.A., Inc.</t>
+  </si>
+  <si>
+    <t>Generos</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Racing</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Adventure</t>
+  </si>
+  <si>
+    <t>Casual</t>
+  </si>
+  <si>
+    <t>SUNSET GAMES</t>
+  </si>
+  <si>
+    <t>SmiteWorks USA, LLC</t>
+  </si>
+  <si>
+    <t>STEAM0082987612</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -273,6 +339,20 @@
       <sz val="12"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -359,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,6 +461,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,55 +479,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>591696</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>86189</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{818CBF45-15AE-0230-0D45-B5881320B638}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="8211696" cy="3324689"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,7 +685,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -958,15 +992,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3ED85D-20F3-4304-81A9-6C0DE1D7A778}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1280</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>12690</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>508600</v>
+      </c>
+      <c r="B4">
+        <v>7.6561198211054592E+16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>343170</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>746620</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Optimizacion de funcion UserforGenre
</commit_message>
<xml_diff>
--- a/Bases de datos/Diccionario de Datos STEAM.xlsx
+++ b/Bases de datos/Diccionario de Datos STEAM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documentos\Mai\Henry\Cursado\P.I. 1\Bases de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6030E9-A82C-45C4-82C5-F3B0561A786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCE6885-DD08-4CD1-B4BB-02E88E318848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -452,6 +452,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,9 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +684,7 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
@@ -696,11 +696,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -866,11 +866,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -921,11 +921,11 @@
       <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3ED85D-20F3-4304-81A9-6C0DE1D7A778}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1032,7 +1032,7 @@
       <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="9" t="s">
         <v>73</v>
       </c>
       <c r="E2">
@@ -1043,13 +1043,13 @@
       <c r="A3">
         <v>12690</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E3">
@@ -1077,13 +1077,13 @@
       <c r="A5">
         <v>343170</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="9" t="s">
         <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>77</v>
       </c>
       <c r="E5">
@@ -1094,7 +1094,7 @@
       <c r="A6">
         <v>746620</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>66</v>
       </c>
       <c r="C6" t="s">
@@ -1105,7 +1105,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C7" t="s">

</xml_diff>

<commit_message>
Actualización de modelo ML
</commit_message>
<xml_diff>
--- a/Bases de datos/Diccionario de Datos STEAM.xlsx
+++ b/Bases de datos/Diccionario de Datos STEAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documentos\Mai\Henry\Cursado\P.I. 1\Bases de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCE6885-DD08-4CD1-B4BB-02E88E318848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A4271F8-2E9E-4741-9523-FEC34A5FB9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>steam_games.gz.json</t>
   </si>
@@ -279,20 +279,17 @@
     <t>Casual</t>
   </si>
   <si>
-    <t>SUNSET GAMES</t>
-  </si>
-  <si>
-    <t>SmiteWorks USA, LLC</t>
-  </si>
-  <si>
-    <t>STEAM0082987612</t>
+    <t>DATOS DE PRUEBAS PARA FUNCIONES Y MODELO DE ML</t>
+  </si>
+  <si>
+    <t>76561198211054600</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -341,7 +338,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -349,13 +355,13 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,8 +380,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -435,11 +453,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,9 +485,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,6 +494,19 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,11 +739,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -866,11 +909,11 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -921,11 +964,11 @@
       <c r="A22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -992,129 +1035,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3ED85D-20F3-4304-81A9-6C0DE1D7A778}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="15">
         <v>1280</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D3" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="15">
         <v>2002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
         <v>12690</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="15">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>508600</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="15">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="15">
+        <v>343170</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3">
-        <v>2003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>508600</v>
-      </c>
-      <c r="B4">
-        <v>7.6561198211054592E+16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>343170</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="D6" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E5">
+      <c r="E6" s="15">
         <v>2012</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
         <v>746620</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B7" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>79</v>
+      <c r="E7" s="15">
+        <v>2008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>